<commit_message>
ensure that the read sheet data has their own tests
</commit_message>
<xml_diff>
--- a/examples/c73_crud_sheets/3_sheets_acb.xlsx
+++ b/examples/c73_crud_sheets/3_sheets_acb.xlsx
@@ -9,32 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" xr2:uid="{615D1CF1-C47D-544B-AFEE-036542D0EAD3}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
-    <sheet name="c" sheetId="3" r:id="rId2"/>
-    <sheet name="b" sheetId="2" r:id="rId3"/>
+    <sheet name="c" sheetId="2" r:id="rId2"/>
+    <sheet name="b" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>b</t>
-  </si>
   <si>
     <t>a</t>
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -385,10 +380,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7EF622-7072-A84A-9658-ED8AA201789D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -402,8 +415,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10AEC5B-EF2F-7648-BCC5-8E239DAEE423}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -418,22 +431,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6DAA3B-3AE5-EF4E-8129-C0AED2CF813F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>